<commit_message>
Readme file updated and some alignment changes
</commit_message>
<xml_diff>
--- a/Testing_inspirationalquotesui.xlsx
+++ b/Testing_inspirationalquotesui.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gopi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSAssesments\InspirationalQuotesAssesment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13D9BCD-BE5E-49C7-A0E5-CC041EA7CAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246EBFBC-8831-430F-AE73-489B55974CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBF135F1-D89D-4449-BB55-2CDE2D7E1977}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>Action</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Submitting Empty Fields</t>
-  </si>
-  <si>
     <t>Submitting with required fields empty.</t>
   </si>
   <si>
@@ -199,6 +196,12 @@
   </si>
   <si>
     <t>Quotes with tags should exactly contains life</t>
+  </si>
+  <si>
+    <t>Submitting Empty Fields(-)</t>
+  </si>
+  <si>
+    <t>No Results Found(-)</t>
   </si>
 </sst>
 </file>
@@ -344,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -384,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -490,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -632,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D50DB2-E614-4A75-8F5E-6DFC4DAF1936}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +661,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -666,7 +669,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -684,7 +687,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -695,13 +698,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
@@ -712,13 +715,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>1</v>
@@ -729,13 +732,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1</v>
@@ -746,13 +749,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -763,13 +766,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -778,7 +781,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -789,13 +792,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -806,13 +809,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
@@ -823,13 +826,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>1</v>
@@ -840,13 +843,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>1</v>
@@ -860,10 +863,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>1</v>
@@ -872,7 +875,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -883,13 +886,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>1</v>
@@ -900,13 +903,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>1</v>
@@ -917,13 +920,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1</v>
@@ -934,13 +937,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>1</v>
@@ -951,13 +954,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1</v>
@@ -968,13 +971,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>1</v>

</xml_diff>